<commit_message>
added 2 more tasks -> own listview and own array
</commit_message>
<xml_diff>
--- a/Funkciók_listája.xlsx
+++ b/Funkciók_listája.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1_My Stuff\Dokumentumok\iskola\EKE PTI\5.félév\Mobilprogramozás 1\Mobilprog1Beadando-OOHQ3E\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gabor\Desktop\Mobilprog1Beadando-OOHQ3E\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C2B0846-C6FA-4DF9-B719-89AC722760D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7285ADFA-18FC-4A92-9EB7-66561DE11FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1565,7 +1565,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B21" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.33203125" defaultRowHeight="19.95" customHeight="1"/>
@@ -1735,7 +1735,7 @@
         <v>0.25</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="36" customHeight="1">
@@ -1843,7 +1843,7 @@
       </c>
       <c r="B25" s="7">
         <f>SUMIF(C3:C24,Munka1!A2,B3:B24)</f>
-        <v>4</v>
+        <v>4.25</v>
       </c>
       <c r="C25" s="8"/>
     </row>

</xml_diff>